<commit_message>
Multiple users can be added to the database, each with their own set of attendance dates.
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheets/database_input_deluxe.xlsx
+++ b/src/test/resources/ExcelSheets/database_input_deluxe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="108" windowWidth="12420" windowHeight="8232" activeTab="3"/>
+    <workbookView xWindow="192" yWindow="108" windowWidth="12420" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="NewUsers" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
@@ -35,12 +35,6 @@
     <t>batchType</t>
   </si>
   <si>
-    <t>attendance</t>
-  </si>
-  <si>
-    <t>tasks</t>
-  </si>
-  <si>
     <t>userRole</t>
   </si>
   <si>
@@ -149,10 +143,37 @@
     <t>I'm carrying the will</t>
   </si>
   <si>
-    <t>02/03/2017</t>
-  </si>
-  <si>
-    <t>01/22/2017</t>
+    <t>graduationDate</t>
+  </si>
+  <si>
+    <t>01/02/2017</t>
+  </si>
+  <si>
+    <t>01/06/2017</t>
+  </si>
+  <si>
+    <t>01/16/2017</t>
+  </si>
+  <si>
+    <t>01/17/2017</t>
+  </si>
+  <si>
+    <t>01/19/2017</t>
+  </si>
+  <si>
+    <t>01/18/2017</t>
+  </si>
+  <si>
+    <t>note2</t>
+  </si>
+  <si>
+    <t>note3</t>
+  </si>
+  <si>
+    <t>note4</t>
+  </si>
+  <si>
+    <t>note5</t>
   </si>
 </sst>
 </file>
@@ -196,15 +217,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -514,7 +537,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -549,7 +572,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -557,10 +580,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -568,10 +591,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -579,10 +602,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -590,10 +613,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -601,41 +624,42 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
+      <c r="A9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="6" t="s">
-        <v>29</v>
+      <c r="A12" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -646,11 +670,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -658,8 +680,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
+      <c r="A1" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -702,43 +724,48 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>13</v>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>14</v>
+      <c r="A8" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -748,21 +775,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
+      <c r="A1" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -781,55 +810,84 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>43</v>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>14</v>
+      <c r="A8" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -840,21 +898,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.5546875" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
+      <c r="A1" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -873,55 +933,84 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>44</v>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="b">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>14</v>
+      <c r="A8" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -934,7 +1023,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -943,8 +1032,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="6" t="s">
-        <v>30</v>
+      <c r="A1" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -975,53 +1064,53 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="6" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="4" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="5" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4" t="s">
+    <row r="10" spans="1:10">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4" t="s">
+    <row r="11" spans="1:10">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4" t="s">
+    <row r="12" spans="1:10">
+      <c r="A12" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>